<commit_message>
Backpack Prediction Additional Submissions
Did more submissions this evening, trying out the normalized price again without id overfitting issue.
</commit_message>
<xml_diff>
--- a/Kaggle/Backpack Challenge/2025 02 17 Backpack Prediction Challenge Help File.xlsx
+++ b/Kaggle/Backpack Challenge/2025 02 17 Backpack Prediction Challenge Help File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ironm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ironm\Documents\GitHub\AnalyticsProjects\Kaggle\Backpack Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923BA94A-E911-4BBD-8ED4-2B10B4311C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACEC66C-DB94-465C-836C-F63D2B546E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33480" yWindow="2685" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{79973EF0-639F-49B0-91AA-8D4655D8820B}"/>
+    <workbookView xWindow="2170" yWindow="2060" windowWidth="21300" windowHeight="13030" activeTab="1" xr2:uid="{79973EF0-639F-49B0-91AA-8D4655D8820B}"/>
   </bookViews>
   <sheets>
     <sheet name="Train Data Set" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="124">
   <si>
     <t>id</t>
   </si>
@@ -394,13 +394,31 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Submission 17</t>
+  </si>
+  <si>
+    <t>Trial 1 Redo</t>
+  </si>
+  <si>
+    <t>Submission 18</t>
+  </si>
+  <si>
+    <t>Submission 19</t>
+  </si>
+  <si>
+    <t>Vote with best 3, maybe best 4</t>
+  </si>
+  <si>
+    <t>Try stacking regressor best 3 or 4 with vote as guide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,6 +450,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -477,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -538,6 +563,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1324,20 +1362,20 @@
       <selection activeCell="C26" sqref="C26:E77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="36.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="14.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="36.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="3"/>
+    <col min="6" max="6" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="14.453125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1367,7 +1405,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>9</v>
       </c>
@@ -1403,7 +1441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>4</v>
       </c>
@@ -1439,7 +1477,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <v>10</v>
       </c>
@@ -1475,7 +1513,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <v>0</v>
       </c>
@@ -1511,7 +1549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -1547,7 +1585,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -1583,7 +1621,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -1619,7 +1657,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>1</v>
       </c>
@@ -1655,7 +1693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -1691,7 +1729,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>7</v>
       </c>
@@ -1727,7 +1765,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -1763,12 +1801,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1776,7 +1814,7 @@
         <v>53314</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1789,45 +1827,45 @@
         <v>1.0728701654349702</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C22" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="11"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="11"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="11"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="11"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" s="11"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="11"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" s="11"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="11"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="11"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="11"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="11"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="11"/>
     </row>
   </sheetData>
@@ -1839,888 +1877,995 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B33E58-7A7B-4424-8963-52E76A246AB0}">
-  <dimension ref="C1:K68"/>
+  <dimension ref="C1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="39.54296875" customWidth="1"/>
+    <col min="6" max="6" width="32.54296875" customWidth="1"/>
+    <col min="7" max="7" width="35.7265625" customWidth="1"/>
+    <col min="8" max="8" width="35.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E1">
-        <f>AVERAGE(E19,E26,E33,E40,E47,E54)</f>
+    <row r="1" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="F1">
+        <f>AVERAGE(F19,F26,F33,F40,F47,F54)</f>
         <v>39.141991666666662</v>
       </c>
-      <c r="F1">
-        <f>AVERAGE(F12,F19,F26,F33,F40,F47,F54)</f>
+      <c r="G1">
+        <f>AVERAGE(G12,G19,G26,G33,G40,G47,G54)</f>
         <v>39.144141428571423</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>102</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>76</v>
       </c>
       <c r="G3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
       <c r="D4" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" t="s">
         <v>86</v>
       </c>
-      <c r="F4" t="s">
-        <v>103</v>
+      <c r="F4" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="G4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
       <c r="D5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" s="14"/>
+      <c r="H5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1"/>
       <c r="E7" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D8" s="20">
         <v>0.116194014789763</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="23">
+        <v>0.58082096171623299</v>
+      </c>
+      <c r="F8" s="11">
         <v>39.017954238669297</v>
       </c>
-      <c r="F8" s="11">
+      <c r="G8" s="11">
         <v>39.0216336581368</v>
       </c>
-      <c r="G8" s="11">
+      <c r="H8" s="11">
         <v>38.917643507935303</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="1">
         <v>1.34104024770474E-2</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="23">
+        <v>0.33554159755355001</v>
+      </c>
+      <c r="F9" s="11">
         <v>1522.2318406657801</v>
       </c>
-      <c r="F9" s="11">
+      <c r="G9" s="11">
         <v>1522.7486459230299</v>
       </c>
-      <c r="G9" s="11">
+      <c r="H9" s="11">
         <v>1514.9659746011</v>
       </c>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="1">
         <v>9.6467522080412305E-4</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="23">
+        <v>9.9027927640637993E-4</v>
+      </c>
+      <c r="F10" s="11">
         <v>1.0122945971016101E-3</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G10" s="11">
         <v>6.7313331805485201E-4</v>
       </c>
-      <c r="G10" s="11">
+      <c r="H10" s="11">
         <v>9.2237562848085299E-4</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>78</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="11">
+      <c r="E12" s="23">
+        <v>40.410710000000002</v>
+      </c>
+      <c r="F12" s="1">
+        <v>39.140689999999999</v>
+      </c>
+      <c r="G12" s="11">
         <v>39.147370000000002</v>
       </c>
-      <c r="G12" s="11">
+      <c r="H12" s="11">
         <v>39.147579999999998</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="25"/>
+      <c r="F13" s="3"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="26"/>
+      <c r="F14" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="19">
         <v>0.58088827244361796</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="24"/>
+      <c r="F15" s="11">
         <v>39.020644119963499</v>
       </c>
-      <c r="F15" s="11">
+      <c r="G15" s="11">
         <v>39.0177937588088</v>
       </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="11">
         <v>0.33560429316285301</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="24"/>
+      <c r="F16" s="11">
         <v>1522.39954590003</v>
       </c>
-      <c r="F16" s="11">
+      <c r="G16" s="11">
         <v>1521.70545310844</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I16" s="11"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D17" s="11">
         <v>8.0361531701422795E-4</v>
       </c>
-      <c r="E17" s="11">
+      <c r="F17" s="11">
         <v>9.0223549659296199E-4</v>
       </c>
-      <c r="F17" s="11">
+      <c r="G17" s="11">
         <v>1.3577444057399899E-3</v>
       </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>87</v>
-      </c>
+      <c r="E18" s="11"/>
       <c r="F18" s="11" t="s">
         <v>87</v>
       </c>
       <c r="G18" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="1">
+      <c r="E19" s="3"/>
+      <c r="F19" s="1">
         <v>39.145299999999999</v>
       </c>
-      <c r="F19" s="11">
+      <c r="G19" s="11">
         <v>39.14528</v>
       </c>
-      <c r="H19" s="11"/>
       <c r="I19" s="11"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="11"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E20" s="25"/>
+      <c r="F20" s="3"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C21" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="23"/>
+      <c r="F21" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="G21" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C22" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D22" s="19">
         <v>0.58083435030983099</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="24"/>
+      <c r="F22" s="11">
         <v>39.0168723725752</v>
       </c>
-      <c r="F22" s="11">
+      <c r="G22" s="11">
         <v>39.0126681088827</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="1"/>
+      <c r="L22" s="11"/>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="11">
         <v>0.33539213327475198</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="24"/>
+      <c r="F23" s="11">
         <v>1521.4458602570201</v>
       </c>
-      <c r="F23" s="11">
+      <c r="G23" s="11">
         <v>1520.8887946960499</v>
       </c>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="11">
         <v>1.4352800408683399E-3</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="24"/>
+      <c r="F24" s="11">
         <v>1.52810614699583E-3</v>
       </c>
-      <c r="F24" s="11">
+      <c r="G24" s="11">
         <v>1.8936888602544199E-3</v>
       </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="K25" s="11"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="E26" s="1">
+      <c r="E26" s="25"/>
+      <c r="F26" s="1">
         <v>39.135240000000003</v>
       </c>
-      <c r="F26" s="11">
+      <c r="G26" s="11">
         <v>39.131610000000002</v>
       </c>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="1"/>
-      <c r="I27" s="11" t="s">
+      <c r="E27" s="25"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="1"/>
+      <c r="J27" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C28" s="4" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="G28" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="K28" s="11"/>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H28" s="11"/>
+      <c r="L28" s="11"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D29" s="19">
         <v>0.58082139182333503</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="23">
+        <v>0.58082101544916398</v>
+      </c>
+      <c r="F29" s="11">
         <v>39.017898447347903</v>
       </c>
-      <c r="F29" s="11">
+      <c r="G29" s="11">
         <v>39.021606003854203</v>
       </c>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="11">
         <v>0.335545291405974</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="23">
+        <v>0.33554144700342797</v>
+      </c>
+      <c r="F30" s="11">
         <v>1522.23220172521</v>
       </c>
-      <c r="F30" s="11">
+      <c r="G30" s="11">
         <v>1522.7459193140401</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C31" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D31" s="11">
         <v>9.7928155062565404E-4</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E31" s="23">
+        <v>9.9072751005912997E-4</v>
+      </c>
+      <c r="F31" s="11">
         <v>1.01205764637901E-3</v>
       </c>
-      <c r="F31" s="11">
+      <c r="G31" s="11">
         <v>6.7492269650948301E-4</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="11"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C32" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>94</v>
+      <c r="E32" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G32" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C33" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D33" s="3"/>
-      <c r="E33" s="1">
+      <c r="E33" s="23">
+        <v>40.410769999999999</v>
+      </c>
+      <c r="F33" s="1">
         <v>39.140650000000001</v>
       </c>
-      <c r="F33" s="11">
+      <c r="G33" s="11">
         <v>39.147320000000001</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+      <c r="F34" s="3"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C35" s="4" t="s">
         <v>56</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="22"/>
+      <c r="F35" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="G35" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="H35" s="11"/>
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="11"/>
+      <c r="L35" s="11"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C36" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D36" s="19">
         <v>0.58101090219180196</v>
       </c>
-      <c r="E36" s="11">
+      <c r="F36" s="11">
         <v>39.025520124509903</v>
       </c>
-      <c r="F36" s="11">
+      <c r="G36" s="11">
         <v>39.0319277160336</v>
       </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C37" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D37" s="11">
         <v>0.33575480917858302</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E37" s="1"/>
+      <c r="F37" s="11">
         <v>1522.64719503418</v>
       </c>
-      <c r="F37" s="11">
+      <c r="G37" s="11">
         <v>1523.0605960355299</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="11"/>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+      <c r="J37" s="11"/>
+      <c r="L37" s="1"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C38" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D38" s="11">
         <v>3.5548321078593398E-4</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="22"/>
+      <c r="F38" s="11">
         <v>7.3971200072264699E-4</v>
       </c>
-      <c r="F38" s="11">
+      <c r="G38" s="11">
         <v>4.68411331061791E-4</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="K38" s="11"/>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="11"/>
+      <c r="L38" s="11"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C39" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="F39" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="H39" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C40" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="1">
+      <c r="E40" s="25"/>
+      <c r="F40" s="1">
         <v>39.153260000000003</v>
       </c>
-      <c r="F40" s="11">
+      <c r="G40" s="11">
         <v>39.157820000000001</v>
       </c>
-      <c r="H40" s="11"/>
       <c r="I40" s="11"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="11"/>
+      <c r="L40" s="1"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="H41" s="11"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="3"/>
       <c r="I41" s="11"/>
-      <c r="K41" s="11"/>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="11"/>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C42" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="G42" s="17" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D43" s="19">
         <v>0.58096515299738505</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43" s="24"/>
+      <c r="F43" s="11">
         <v>39.020756154857601</v>
       </c>
-      <c r="F43" s="11">
+      <c r="G43" s="11">
         <v>39.0179361260153</v>
       </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="11"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+      <c r="J43" s="11"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D44" s="11">
         <v>0.335406950261387</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E44" s="24"/>
+      <c r="F44" s="11">
         <v>1522.19982681652</v>
       </c>
-      <c r="F44" s="11">
+      <c r="G44" s="11">
         <v>1521.5792147500099</v>
       </c>
-      <c r="H44" s="11"/>
-      <c r="K44" s="11"/>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I44" s="11"/>
+      <c r="L44" s="11"/>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D45" s="11">
         <v>1.3911653505045401E-3</v>
       </c>
-      <c r="E45" s="11">
+      <c r="E45" s="24"/>
+      <c r="F45" s="11">
         <v>1.0333041706448399E-3</v>
       </c>
-      <c r="F45" s="11">
+      <c r="G45" s="11">
         <v>1.44059024081455E-3</v>
       </c>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C46" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="G46" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="H46" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="11"/>
-    </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I46" s="1"/>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C47" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D47" s="3"/>
-      <c r="E47" s="1">
+      <c r="E47" s="25"/>
+      <c r="F47" s="1">
         <v>39.142229999999998</v>
       </c>
-      <c r="F47" s="11">
+      <c r="G47" s="11">
         <v>39.145589999999999</v>
       </c>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="1"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E48" s="25"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="1"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C49" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="23"/>
+      <c r="F49" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="G49" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="11"/>
-    </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C50" s="1" t="s">
         <v>85</v>
       </c>
       <c r="D50" s="19">
         <v>0.58075021802237103</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="24"/>
+      <c r="F50" s="11">
         <v>39.014648741618402</v>
       </c>
-      <c r="F50" s="11">
+      <c r="G50" s="11">
         <v>39.012793974019402</v>
       </c>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C51" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D51" s="11">
         <v>0.33534590319375202</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E51" s="24"/>
+      <c r="F51" s="11">
         <v>1521.6167300279401</v>
       </c>
-      <c r="F51" s="11">
+      <c r="G51" s="11">
         <v>1521.29734871697</v>
       </c>
-      <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C52" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D52" s="11">
         <v>1.5729210983289599E-3</v>
       </c>
-      <c r="E52" s="11">
+      <c r="E52" s="24"/>
+      <c r="F52" s="11">
         <v>1.41597027136408E-3</v>
       </c>
-      <c r="F52" s="11">
+      <c r="G52" s="11">
         <v>1.6255690949281601E-3</v>
       </c>
-      <c r="I52" s="11"/>
-    </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C53" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E53" s="11" t="s">
-        <v>63</v>
-      </c>
+      <c r="E53" s="24"/>
       <c r="F53" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="I53" s="12"/>
-    </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C54" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D54" s="3"/>
-      <c r="E54" s="1">
+      <c r="E54" s="25"/>
+      <c r="F54" s="1">
         <v>39.135269999999998</v>
       </c>
-      <c r="F54" s="11">
+      <c r="G54" s="11">
         <v>39.134</v>
       </c>
-      <c r="I54" s="11"/>
-    </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="11"/>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E55" s="25"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="11"/>
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C56" s="13" t="s">
         <v>67</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="11"/>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E56" s="23"/>
+      <c r="F56" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C57" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D57" s="11">
         <v>0.33534590319375202</v>
       </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="11"/>
-      <c r="I57" s="11"/>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E57" s="24"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C58" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D58" s="11">
         <v>1.5729210983289599E-3</v>
       </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="11"/>
-      <c r="I58" s="11"/>
-    </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E58" s="24"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C59" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="E60" s="3"/>
-      <c r="F60" s="1"/>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E59" s="25"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="E60" s="26"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.35">
       <c r="D61" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="11"/>
-      <c r="I61" s="11"/>
-    </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E61" s="26"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C62" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E62" s="3"/>
-      <c r="I62" s="12"/>
-    </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E62" s="23"/>
+      <c r="F62" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G62" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C63" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D63" s="11">
         <v>0.57915372246227903</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E63" s="24"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C64" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D64" s="11">
         <v>1.3551876532552601E-3</v>
       </c>
-      <c r="F64" s="11"/>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E64" s="24"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D65" s="15">
         <v>40.279640000000001</v>
       </c>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F67" s="11"/>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="F68" s="12"/>
+      <c r="E65" s="15"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="G68" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>